<commit_message>
DOM change Nov10 ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC16_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC16_Verify_UserRegistration.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="TC16_Verify_UserRegistration" sheetId="1" r:id="rId1"/>
+    <sheet name="TC23_Verify_UserRegistration" sheetId="1" r:id="rId1"/>
     <sheet name="Testdata" sheetId="12" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t>TestCase</t>
   </si>
@@ -53,6 +58,9 @@
     <t>ENTERTEXT</t>
   </si>
   <si>
+    <t>TC23_Verify_UserRegistration</t>
+  </si>
+  <si>
     <t>RegisterButton</t>
   </si>
   <si>
@@ -119,12 +127,6 @@
     <t>ExistingaccNObutton</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
     <t>CLICK_JS</t>
   </si>
   <si>
@@ -152,9 +154,6 @@
     <t>Button</t>
   </si>
   <si>
-    <t>Profile</t>
-  </si>
-  <si>
     <t>EleType1</t>
   </si>
   <si>
@@ -173,7 +172,10 @@
     <t>MyaccountSecRegisteredUser</t>
   </si>
   <si>
-    <t>TC16_Verify_UserRegistration</t>
+    <t>SignOut</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
@@ -254,7 +256,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,17 +606,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -621,7 +625,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -636,7 +640,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -648,9 +652,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -659,342 +663,360 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>28</v>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>28</v>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1008,7 +1030,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1030,111 +1052,111 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3">
         <v>75230</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1148,6 +1170,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1156,7 +1184,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1353,13 +1381,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1367,7 +1398,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1384,21 +1415,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ECTEST- update for support
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC16_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC16_Verify_UserRegistration.xlsx
@@ -609,7 +609,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1176,15 +1176,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1381,6 +1372,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
@@ -1391,14 +1391,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1415,4 +1407,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>